<commit_message>
Practica 4 menos el punto 25
</commit_message>
<xml_diff>
--- a/PRACTICAS/PRACTICA_4/Punto12.xlsx
+++ b/PRACTICAS/PRACTICA_4/Punto12.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
-  <workbookPr showObjects="none" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Agus\Escritorio\Facultad\2DO AÑO\2do_Semestre\ISO\PRACTICAS\PRACTICA_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AF0FA6-C3A0-4E5C-8111-38574F6D9274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F12AC86-6933-49EF-AE70-9A0161C8D25C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CDD4E7AF-A631-4D77-AD2C-28A26D27A9FE}"/>
   </bookViews>
@@ -119,27 +119,20 @@
     <t>Aux Qeue</t>
   </si>
   <si>
-    <t>11.8</t>
-  </si>
-  <si>
-    <t>7.6</t>
+    <t>12.4</t>
+  </si>
+  <si>
+    <t>8.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -163,6 +156,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -216,9 +210,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -234,15 +227,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Accent5" xfId="1" builtinId="45"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -555,20 +547,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB3275D-6D27-466C-A52D-F344A9C235B1}">
-  <dimension ref="A1:AC9"/>
+  <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="29" width="4.7109375" customWidth="1"/>
+    <col min="6" max="31" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -647,15 +639,21 @@
       <c r="Z1" s="2">
         <v>20</v>
       </c>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2" t="s">
+      <c r="AA1" s="2">
+        <v>21</v>
+      </c>
+      <c r="AB1" s="2">
+        <v>22</v>
+      </c>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -675,17 +673,17 @@
       <c r="G2" s="2">
         <v>2</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="2">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2">
         <v>3</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -701,14 +699,16 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
-      <c r="AB2" s="2">
-        <v>6</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>2</v>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2">
+        <v>7</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -725,51 +725,55 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2">
-        <v>2</v>
-      </c>
-      <c r="J3" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="2">
+      <c r="N3" s="2"/>
+      <c r="O3" s="2">
         <v>3</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>4</v>
       </c>
-      <c r="Q3" s="2">
-        <v>5</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
+      <c r="W3" s="2">
+        <v>5</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="AA3" s="2"/>
-      <c r="AB3" s="2">
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE3" s="2">
         <v>13</v>
       </c>
-      <c r="AC3" s="2">
-        <v>7</v>
-      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -789,38 +793,40 @@
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2">
+      <c r="L4" s="2"/>
+      <c r="M4" s="2">
         <v>1</v>
       </c>
-      <c r="M4" s="2">
-        <v>2</v>
-      </c>
-      <c r="N4" s="2"/>
+      <c r="N4" s="2">
+        <v>2</v>
+      </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="R4" s="2">
+        <v>3</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
-      <c r="W4" s="2">
-        <v>3</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
-      <c r="AB4" s="2">
-        <v>16</v>
-      </c>
-      <c r="AC4" s="2">
-        <v>12</v>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2">
+        <v>11</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -845,43 +851,45 @@
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="2">
+      <c r="O5" s="2"/>
+      <c r="P5" s="2">
         <v>1</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="Q5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="R5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="2">
-        <v>2</v>
-      </c>
-      <c r="S5" s="2">
+      <c r="S5" s="2"/>
+      <c r="T5" s="2">
+        <v>2</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2">
         <v>3</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="Y5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="U5" s="2">
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2">
         <v>4</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="AB5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2">
-        <v>11</v>
-      </c>
-      <c r="AC5" s="2">
-        <v>6</v>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2">
+        <v>17</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -910,25 +918,27 @@
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
+      <c r="U6" s="2">
+        <v>1</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
-      <c r="Y6" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
-      <c r="AB6" s="2">
-        <v>13</v>
-      </c>
-      <c r="AC6" s="2">
-        <v>11</v>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2">
+        <v>8</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -940,30 +950,36 @@
         <v>26</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>1</v>
       </c>
-      <c r="G7" s="6">
-        <v>2</v>
-      </c>
-      <c r="H7" s="6">
+      <c r="G7" s="5">
+        <v>2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
         <v>3</v>
       </c>
-      <c r="I7" s="6">
-        <v>2</v>
-      </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
+        <v>2</v>
+      </c>
+      <c r="K7" s="5">
         <v>4</v>
       </c>
-      <c r="K7" s="6">
+      <c r="L7" s="5">
         <v>3</v>
       </c>
-      <c r="L7" s="6">
+      <c r="M7" s="5">
         <v>5</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="N7" s="5">
+        <v>2</v>
+      </c>
+      <c r="O7" s="5">
+        <v>4</v>
+      </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -976,14 +992,16 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
-      <c r="AB7" s="2" t="s">
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AC7" s="2" t="s">
+      <c r="AE7" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -991,21 +1009,19 @@
         <v>27</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>2</v>
-      </c>
-      <c r="H8" s="6">
+      <c r="F8" s="5">
+        <v>2</v>
+      </c>
+      <c r="G8" s="5">
         <v>4</v>
       </c>
-      <c r="I8" s="6">
-        <v>2</v>
-      </c>
-      <c r="J8" s="6">
+      <c r="H8" s="5">
+        <v>2</v>
+      </c>
+      <c r="I8" s="5">
         <v>4</v>
       </c>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1025,8 +1041,10 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>

</xml_diff>

<commit_message>
correccion (no me acuerdo que hice en el 6)
</commit_message>
<xml_diff>
--- a/PRACTICAS/PRACTICA_4/Punto12.xlsx
+++ b/PRACTICAS/PRACTICA_4/Punto12.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Agus\Escritorio\Facultad\2DO AÑO\2do_Semestre\ISO\PRACTICAS\PRACTICA_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F12AC86-6933-49EF-AE70-9A0161C8D25C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137E36A2-DDE1-4C21-BBAC-40BC54478338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CDD4E7AF-A631-4D77-AD2C-28A26D27A9FE}"/>
   </bookViews>
@@ -119,10 +119,10 @@
     <t>Aux Qeue</t>
   </si>
   <si>
-    <t>12.4</t>
-  </si>
-  <si>
-    <t>8.2</t>
+    <t>11.6</t>
+  </si>
+  <si>
+    <t>7.4</t>
   </si>
 </sst>
 </file>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB3275D-6D27-466C-A52D-F344A9C235B1}">
-  <dimension ref="A1:AE9"/>
+  <dimension ref="A1:AD9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +560,7 @@
     <col min="6" max="31" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -642,18 +642,15 @@
       <c r="AA1" s="2">
         <v>21</v>
       </c>
-      <c r="AB1" s="2">
-        <v>22</v>
-      </c>
-      <c r="AC1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="AD1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -677,13 +674,13 @@
         <v>10</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2">
+      <c r="J2" s="2">
         <v>3</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -700,15 +697,14 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
+      <c r="AC2" s="2">
+        <v>6</v>
+      </c>
       <c r="AD2" s="2">
-        <v>7</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -725,55 +721,52 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="I3" s="2">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2">
+      <c r="N3" s="2">
         <v>3</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="P3" s="2">
         <v>4</v>
       </c>
+      <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2">
+      <c r="V3" s="2">
         <v>5</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
+      <c r="AC3" s="2">
+        <v>18</v>
+      </c>
       <c r="AD3" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE3" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -793,22 +786,22 @@
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
       <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="N4" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2">
+      <c r="Q4" s="2">
         <v>3</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
@@ -818,15 +811,14 @@
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
+      <c r="AC4" s="2">
+        <v>10</v>
+      </c>
       <c r="AD4" s="2">
-        <v>11</v>
-      </c>
-      <c r="AE4" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -851,45 +843,44 @@
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2">
+      <c r="O5" s="2">
         <v>1</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2">
-        <v>2</v>
-      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2">
+        <v>2</v>
+      </c>
+      <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2">
+      <c r="W5" s="2">
         <v>3</v>
       </c>
-      <c r="Y5" s="6" t="s">
+      <c r="X5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2">
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2">
         <v>4</v>
       </c>
-      <c r="AB5" s="2" t="s">
+      <c r="AA5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AC5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2">
+        <v>16</v>
+      </c>
       <c r="AD5" s="2">
-        <v>17</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -917,28 +908,27 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2">
+      <c r="T6" s="2">
         <v>1</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="U6" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="V6" s="2"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
+      <c r="AC6" s="2">
+        <v>8</v>
+      </c>
       <c r="AD6" s="2">
-        <v>8</v>
-      </c>
-      <c r="AE6" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -993,15 +983,14 @@
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
+      <c r="AC7" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="AD7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE7" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1042,9 +1031,8 @@
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>

</xml_diff>